<commit_message>
added script to input random data into excel file
</commit_message>
<xml_diff>
--- a/server/Fitness_Records_Hackathon.xlsx
+++ b/server/Fitness_Records_Hackathon.xlsx
@@ -468,6 +468,21 @@
       <c r="D2" t="str">
         <v>Female</v>
       </c>
+      <c r="E2">
+        <v>20.529902773642704</v>
+      </c>
+      <c r="F2">
+        <v>47.831146818906234</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>96.3671244523385</v>
+      </c>
+      <c r="I2">
+        <v>7607</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -482,20 +497,20 @@
       <c r="D3" t="str">
         <v>Male</v>
       </c>
-      <c r="E3" t="str">
-        <v>75</v>
-      </c>
-      <c r="F3" t="str">
-        <v>145</v>
-      </c>
-      <c r="G3" t="str">
+      <c r="E3">
+        <v>69.11079584306997</v>
+      </c>
+      <c r="F3">
+        <v>47.02211153882789</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" t="str">
-        <v>30</v>
-      </c>
-      <c r="I3" t="str">
-        <v>10000</v>
+      <c r="H3">
+        <v>65.3498075807977</v>
+      </c>
+      <c r="I3">
+        <v>9327</v>
       </c>
     </row>
     <row r="4">
@@ -511,6 +526,21 @@
       <c r="D4" t="str">
         <v>Female</v>
       </c>
+      <c r="E4">
+        <v>80.96905550423095</v>
+      </c>
+      <c r="F4">
+        <v>75.67654264296633</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>110.78149129053828</v>
+      </c>
+      <c r="I4">
+        <v>6205</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -525,6 +555,21 @@
       <c r="D5" t="str">
         <v>Male</v>
       </c>
+      <c r="E5">
+        <v>14.428548067269409</v>
+      </c>
+      <c r="F5">
+        <v>80.07189894982348</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>86.67793852664987</v>
+      </c>
+      <c r="I5">
+        <v>782</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -539,6 +584,21 @@
       <c r="D6" t="str">
         <v>Female</v>
       </c>
+      <c r="E6">
+        <v>33.71474718115009</v>
+      </c>
+      <c r="F6">
+        <v>151.87669993655248</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>106.02165076486736</v>
+      </c>
+      <c r="I6">
+        <v>2292</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -553,6 +613,21 @@
       <c r="D7" t="str">
         <v>Male</v>
       </c>
+      <c r="E7">
+        <v>95.38833111021594</v>
+      </c>
+      <c r="F7">
+        <v>161.02921967497815</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>30.039888187841505</v>
+      </c>
+      <c r="I7">
+        <v>8872</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -567,6 +642,21 @@
       <c r="D8" t="str">
         <v>Female</v>
       </c>
+      <c r="E8">
+        <v>42.27250586317437</v>
+      </c>
+      <c r="F8">
+        <v>54.22520139243119</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>38.48622918081815</v>
+      </c>
+      <c r="I8">
+        <v>8908</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -581,6 +671,21 @@
       <c r="D9" t="str">
         <v>Female</v>
       </c>
+      <c r="E9">
+        <v>96.5881854907074</v>
+      </c>
+      <c r="F9">
+        <v>21.617079608274416</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>64.31603511132553</v>
+      </c>
+      <c r="I9">
+        <v>7666</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -595,6 +700,21 @@
       <c r="D10" t="str">
         <v>Male</v>
       </c>
+      <c r="E10">
+        <v>14.712779637107953</v>
+      </c>
+      <c r="F10">
+        <v>76.71955859751716</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>7.262679744390015</v>
+      </c>
+      <c r="I10">
+        <v>7478</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -609,6 +729,21 @@
       <c r="D11" t="str">
         <v>Female</v>
       </c>
+      <c r="E11">
+        <v>31.651054371566765</v>
+      </c>
+      <c r="F11">
+        <v>198.32804386347118</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>58.76965581134836</v>
+      </c>
+      <c r="I11">
+        <v>8398</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -623,6 +758,21 @@
       <c r="D12" t="str">
         <v>Male</v>
       </c>
+      <c r="E12">
+        <v>87.52317780501728</v>
+      </c>
+      <c r="F12">
+        <v>23.35355683125715</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <v>19.938362103891354</v>
+      </c>
+      <c r="I12">
+        <v>9735</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -637,6 +787,21 @@
       <c r="D13" t="str">
         <v>Female</v>
       </c>
+      <c r="E13">
+        <v>36.042601612407445</v>
+      </c>
+      <c r="F13">
+        <v>188.68292169430526</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>37.72459149728553</v>
+      </c>
+      <c r="I13">
+        <v>1812</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -651,6 +816,21 @@
       <c r="D14" t="str">
         <v>Male</v>
       </c>
+      <c r="E14">
+        <v>31.829633535017532</v>
+      </c>
+      <c r="F14">
+        <v>60.6023835522481</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>93.4960322797487</v>
+      </c>
+      <c r="I14">
+        <v>6246</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -665,6 +845,21 @@
       <c r="D15" t="str">
         <v>Female</v>
       </c>
+      <c r="E15">
+        <v>20.546759430112928</v>
+      </c>
+      <c r="F15">
+        <v>115.19265696905876</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>46.79821005293896</v>
+      </c>
+      <c r="I15">
+        <v>9090</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -679,6 +874,21 @@
       <c r="D16" t="str">
         <v>Male</v>
       </c>
+      <c r="E16">
+        <v>0.44500279531718423</v>
+      </c>
+      <c r="F16">
+        <v>147.22636545998918</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>106.78086298856282</v>
+      </c>
+      <c r="I16">
+        <v>3847</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -693,6 +903,21 @@
       <c r="D17" t="str">
         <v>Female</v>
       </c>
+      <c r="E17">
+        <v>13.583214742216555</v>
+      </c>
+      <c r="F17">
+        <v>105.27049955190586</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>9.513142004410389</v>
+      </c>
+      <c r="I17">
+        <v>1796</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18">
@@ -707,6 +932,21 @@
       <c r="D18" t="str">
         <v>Female</v>
       </c>
+      <c r="E18">
+        <v>46.692327327948455</v>
+      </c>
+      <c r="F18">
+        <v>124.81750898966872</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>9.697020685253488</v>
+      </c>
+      <c r="I18">
+        <v>5565</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -721,6 +961,21 @@
       <c r="D19" t="str">
         <v>Male</v>
       </c>
+      <c r="E19">
+        <v>73.05622258305758</v>
+      </c>
+      <c r="F19">
+        <v>89.36002916876436</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>19.89744637290424</v>
+      </c>
+      <c r="I19">
+        <v>520</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -735,6 +990,21 @@
       <c r="D20" t="str">
         <v>Female</v>
       </c>
+      <c r="E20">
+        <v>17.554903581122595</v>
+      </c>
+      <c r="F20">
+        <v>44.2810320350171</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>110.28793694371318</v>
+      </c>
+      <c r="I20">
+        <v>5300</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -749,6 +1019,21 @@
       <c r="D21" t="str">
         <v>Male</v>
       </c>
+      <c r="E21">
+        <v>70.0124367983723</v>
+      </c>
+      <c r="F21">
+        <v>164.76568937581857</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>34.34632787530162</v>
+      </c>
+      <c r="I21">
+        <v>2308</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22">
@@ -763,6 +1048,21 @@
       <c r="D22" t="str">
         <v>Female</v>
       </c>
+      <c r="E22">
+        <v>24.77677227943531</v>
+      </c>
+      <c r="F22">
+        <v>157.9267455566939</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>93.5088421991492</v>
+      </c>
+      <c r="I22">
+        <v>4912</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -777,6 +1077,21 @@
       <c r="D23" t="str">
         <v>Male</v>
       </c>
+      <c r="E23">
+        <v>90.14623595729643</v>
+      </c>
+      <c r="F23">
+        <v>76.2145752588483</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23">
+        <v>59.01242371789677</v>
+      </c>
+      <c r="I23">
+        <v>5693</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24">
@@ -791,6 +1106,21 @@
       <c r="D24" t="str">
         <v>Female</v>
       </c>
+      <c r="E24">
+        <v>88.956297183779</v>
+      </c>
+      <c r="F24">
+        <v>23.95359097817331</v>
+      </c>
+      <c r="G24">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>39.00099012050323</v>
+      </c>
+      <c r="I24">
+        <v>6011</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -805,6 +1135,21 @@
       <c r="D25" t="str">
         <v>Male</v>
       </c>
+      <c r="E25">
+        <v>0.11479606012998467</v>
+      </c>
+      <c r="F25">
+        <v>174.8035019331459</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>84.34251085948131</v>
+      </c>
+      <c r="I25">
+        <v>1786</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26">
@@ -819,6 +1164,21 @@
       <c r="D26" t="str">
         <v>Male</v>
       </c>
+      <c r="E26">
+        <v>63.1428509931643</v>
+      </c>
+      <c r="F26">
+        <v>147.57283190244323</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>75.59504620261319</v>
+      </c>
+      <c r="I26">
+        <v>699</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -833,6 +1193,21 @@
       <c r="D27" t="str">
         <v>Female</v>
       </c>
+      <c r="E27">
+        <v>34.862159640362364</v>
+      </c>
+      <c r="F27">
+        <v>119.09677541440567</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>54.01415745322644</v>
+      </c>
+      <c r="I27">
+        <v>9617</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -847,6 +1222,21 @@
       <c r="D28" t="str">
         <v>Male</v>
       </c>
+      <c r="E28">
+        <v>91.52205508603039</v>
+      </c>
+      <c r="F28">
+        <v>6.843688030885087</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28">
+        <v>54.90497235864534</v>
+      </c>
+      <c r="I28">
+        <v>698</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -861,6 +1251,21 @@
       <c r="D29" t="str">
         <v>Female</v>
       </c>
+      <c r="E29">
+        <v>47.74186755389878</v>
+      </c>
+      <c r="F29">
+        <v>86.40880633733508</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <v>111.29360831297363</v>
+      </c>
+      <c r="I29">
+        <v>4821</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -875,6 +1280,21 @@
       <c r="D30" t="str">
         <v>Male</v>
       </c>
+      <c r="E30">
+        <v>24.235387521226226</v>
+      </c>
+      <c r="F30">
+        <v>50.60172133538852</v>
+      </c>
+      <c r="G30">
+        <v>6</v>
+      </c>
+      <c r="H30">
+        <v>62.08347116138591</v>
+      </c>
+      <c r="I30">
+        <v>5020</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -889,6 +1309,21 @@
       <c r="D31" t="str">
         <v>Female</v>
       </c>
+      <c r="E31">
+        <v>57.400638890317836</v>
+      </c>
+      <c r="F31">
+        <v>178.72259530354344</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <v>2.6087813238325985</v>
+      </c>
+      <c r="I31">
+        <v>6188</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32">
@@ -903,6 +1338,21 @@
       <c r="D32" t="str">
         <v>Male</v>
       </c>
+      <c r="E32">
+        <v>76.4056008488194</v>
+      </c>
+      <c r="F32">
+        <v>54.843189917176936</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>111.8040942835604</v>
+      </c>
+      <c r="I32">
+        <v>7306</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -917,6 +1367,21 @@
       <c r="D33" t="str">
         <v>Female</v>
       </c>
+      <c r="E33">
+        <v>29.78108048852528</v>
+      </c>
+      <c r="F33">
+        <v>45.07390991862583</v>
+      </c>
+      <c r="G33">
+        <v>5</v>
+      </c>
+      <c r="H33">
+        <v>102.61549668697492</v>
+      </c>
+      <c r="I33">
+        <v>4706</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -931,6 +1396,21 @@
       <c r="D34" t="str">
         <v>Female</v>
       </c>
+      <c r="E34">
+        <v>66.91861198518421</v>
+      </c>
+      <c r="F34">
+        <v>172.73230684544595</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>39.06859226350694</v>
+      </c>
+      <c r="I34">
+        <v>2380</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -945,6 +1425,21 @@
       <c r="D35" t="str">
         <v>Male</v>
       </c>
+      <c r="E35">
+        <v>4.131596034102936</v>
+      </c>
+      <c r="F35">
+        <v>136.5890168316129</v>
+      </c>
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <v>96.49091671177575</v>
+      </c>
+      <c r="I35">
+        <v>8612</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -959,6 +1454,21 @@
       <c r="D36" t="str">
         <v>Female</v>
       </c>
+      <c r="E36">
+        <v>41.24235474479501</v>
+      </c>
+      <c r="F36">
+        <v>145.92867038465874</v>
+      </c>
+      <c r="G36">
+        <v>5</v>
+      </c>
+      <c r="H36">
+        <v>10.98826595803473</v>
+      </c>
+      <c r="I36">
+        <v>5459</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -973,6 +1483,21 @@
       <c r="D37" t="str">
         <v>Male</v>
       </c>
+      <c r="E37">
+        <v>10.45696169440693</v>
+      </c>
+      <c r="F37">
+        <v>56.94570186531776</v>
+      </c>
+      <c r="G37">
+        <v>6</v>
+      </c>
+      <c r="H37">
+        <v>47.69623900142076</v>
+      </c>
+      <c r="I37">
+        <v>6008</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38">
@@ -987,6 +1512,21 @@
       <c r="D38" t="str">
         <v>Female</v>
       </c>
+      <c r="E38">
+        <v>68.5430565598673</v>
+      </c>
+      <c r="F38">
+        <v>108.99741027489043</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>119.26526211390326</v>
+      </c>
+      <c r="I38">
+        <v>1337</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39">
@@ -1001,6 +1541,21 @@
       <c r="D39" t="str">
         <v>Male</v>
       </c>
+      <c r="E39">
+        <v>52.028958191566055</v>
+      </c>
+      <c r="F39">
+        <v>107.80406435396822</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>11.589111396907281</v>
+      </c>
+      <c r="I39">
+        <v>2069</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40">
@@ -1015,6 +1570,21 @@
       <c r="D40" t="str">
         <v>Female</v>
       </c>
+      <c r="E40">
+        <v>33.212595865297786</v>
+      </c>
+      <c r="F40">
+        <v>138.7056068031625</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>17.071487429192665</v>
+      </c>
+      <c r="I40">
+        <v>7236</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41">
@@ -1029,6 +1599,21 @@
       <c r="D41" t="str">
         <v>Male</v>
       </c>
+      <c r="E41">
+        <v>20.185407182197366</v>
+      </c>
+      <c r="F41">
+        <v>47.56962564342872</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>60.538540989889775</v>
+      </c>
+      <c r="I41">
+        <v>3053</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42">
@@ -1043,6 +1628,21 @@
       <c r="D42" t="str">
         <v>Female</v>
       </c>
+      <c r="E42">
+        <v>86.48450460401259</v>
+      </c>
+      <c r="F42">
+        <v>168.49370644449183</v>
+      </c>
+      <c r="G42">
+        <v>6</v>
+      </c>
+      <c r="H42">
+        <v>102.3601619255936</v>
+      </c>
+      <c r="I42">
+        <v>3080</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -1057,6 +1657,21 @@
       <c r="D43" t="str">
         <v>Female</v>
       </c>
+      <c r="E43">
+        <v>99.8158147103394</v>
+      </c>
+      <c r="F43">
+        <v>158.2708474065532</v>
+      </c>
+      <c r="G43">
+        <v>6</v>
+      </c>
+      <c r="H43">
+        <v>15.645876314839589</v>
+      </c>
+      <c r="I43">
+        <v>1535</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44">
@@ -1071,6 +1686,21 @@
       <c r="D44" t="str">
         <v>Male</v>
       </c>
+      <c r="E44">
+        <v>72.52034841065984</v>
+      </c>
+      <c r="F44">
+        <v>194.5690013452821</v>
+      </c>
+      <c r="G44">
+        <v>3</v>
+      </c>
+      <c r="H44">
+        <v>54.380363837232295</v>
+      </c>
+      <c r="I44">
+        <v>6004</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45">
@@ -1085,6 +1715,21 @@
       <c r="D45" t="str">
         <v>Female</v>
       </c>
+      <c r="E45">
+        <v>53.711180585303666</v>
+      </c>
+      <c r="F45">
+        <v>26.143412409751534</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+      <c r="H45">
+        <v>23.785179345130505</v>
+      </c>
+      <c r="I45">
+        <v>7821</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46">
@@ -1099,6 +1744,21 @@
       <c r="D46" t="str">
         <v>Male</v>
       </c>
+      <c r="E46">
+        <v>26.88278846176917</v>
+      </c>
+      <c r="F46">
+        <v>44.70629001272175</v>
+      </c>
+      <c r="G46">
+        <v>4</v>
+      </c>
+      <c r="H46">
+        <v>0.27651204398384976</v>
+      </c>
+      <c r="I46">
+        <v>936</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47">
@@ -1113,6 +1773,21 @@
       <c r="D47" t="str">
         <v>Female</v>
       </c>
+      <c r="E47">
+        <v>94.75234625813735</v>
+      </c>
+      <c r="F47">
+        <v>195.8737164612018</v>
+      </c>
+      <c r="G47">
+        <v>5</v>
+      </c>
+      <c r="H47">
+        <v>71.29527375704279</v>
+      </c>
+      <c r="I47">
+        <v>2761</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48">
@@ -1127,6 +1802,21 @@
       <c r="D48" t="str">
         <v>Male</v>
       </c>
+      <c r="E48">
+        <v>66.32321436837914</v>
+      </c>
+      <c r="F48">
+        <v>103.70050480401774</v>
+      </c>
+      <c r="G48">
+        <v>4</v>
+      </c>
+      <c r="H48">
+        <v>29.95842982387768</v>
+      </c>
+      <c r="I48">
+        <v>1233</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49">
@@ -1141,6 +1831,21 @@
       <c r="D49" t="str">
         <v>Female</v>
       </c>
+      <c r="E49">
+        <v>17.199481114381186</v>
+      </c>
+      <c r="F49">
+        <v>178.84738067989662</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>6.178392590946151</v>
+      </c>
+      <c r="I49">
+        <v>2768</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50">
@@ -1155,6 +1860,21 @@
       <c r="D50" t="str">
         <v>Male</v>
       </c>
+      <c r="E50">
+        <v>8.154945032337979</v>
+      </c>
+      <c r="F50">
+        <v>99.30437031457208</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>38.7656337932591</v>
+      </c>
+      <c r="I50">
+        <v>626</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51">
@@ -1169,6 +1889,21 @@
       <c r="D51" t="str">
         <v>Female</v>
       </c>
+      <c r="E51">
+        <v>69.34032380710589</v>
+      </c>
+      <c r="F51">
+        <v>92.05574582947813</v>
+      </c>
+      <c r="G51">
+        <v>6</v>
+      </c>
+      <c r="H51">
+        <v>111.43288770765292</v>
+      </c>
+      <c r="I51">
+        <v>4984</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52">
@@ -1183,6 +1918,21 @@
       <c r="D52" t="str">
         <v>Female</v>
       </c>
+      <c r="E52">
+        <v>37.79430328548086</v>
+      </c>
+      <c r="F52">
+        <v>173.73217951666663</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>5.539812801238844</v>
+      </c>
+      <c r="I52">
+        <v>6941</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53">
@@ -1197,6 +1947,21 @@
       <c r="D53" t="str">
         <v>Male</v>
       </c>
+      <c r="E53">
+        <v>52.17478573100303</v>
+      </c>
+      <c r="F53">
+        <v>94.05729601661163</v>
+      </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
+      <c r="H53">
+        <v>59.19138639249483</v>
+      </c>
+      <c r="I53">
+        <v>2925</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54">
@@ -1211,6 +1976,21 @@
       <c r="D54" t="str">
         <v>Female</v>
       </c>
+      <c r="E54">
+        <v>73.81128707586497</v>
+      </c>
+      <c r="F54">
+        <v>109.40848534004775</v>
+      </c>
+      <c r="G54">
+        <v>3</v>
+      </c>
+      <c r="H54">
+        <v>98.49643933541168</v>
+      </c>
+      <c r="I54">
+        <v>5330</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55">
@@ -1225,6 +2005,21 @@
       <c r="D55" t="str">
         <v>Male</v>
       </c>
+      <c r="E55">
+        <v>61.16852493798073</v>
+      </c>
+      <c r="F55">
+        <v>145.92451287191017</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>17.102764245154223</v>
+      </c>
+      <c r="I55">
+        <v>7283</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56">
@@ -1239,6 +2034,21 @@
       <c r="D56" t="str">
         <v>Female</v>
       </c>
+      <c r="E56">
+        <v>21.136780459815775</v>
+      </c>
+      <c r="F56">
+        <v>8.699095927471268</v>
+      </c>
+      <c r="G56">
+        <v>5</v>
+      </c>
+      <c r="H56">
+        <v>108.28375817170614</v>
+      </c>
+      <c r="I56">
+        <v>2158</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57">
@@ -1253,6 +2063,21 @@
       <c r="D57" t="str">
         <v>Male</v>
       </c>
+      <c r="E57">
+        <v>22.155712962191032</v>
+      </c>
+      <c r="F57">
+        <v>9.061026985666798</v>
+      </c>
+      <c r="G57">
+        <v>6</v>
+      </c>
+      <c r="H57">
+        <v>60.652275211569005</v>
+      </c>
+      <c r="I57">
+        <v>864</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58">
@@ -1267,6 +2092,21 @@
       <c r="D58" t="str">
         <v>Female</v>
       </c>
+      <c r="E58">
+        <v>32.74697980694445</v>
+      </c>
+      <c r="F58">
+        <v>159.76604311330345</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>73.08254650414992</v>
+      </c>
+      <c r="I58">
+        <v>5436</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59">
@@ -1281,6 +2121,21 @@
       <c r="D59" t="str">
         <v>Male</v>
       </c>
+      <c r="E59">
+        <v>34.299496144265795</v>
+      </c>
+      <c r="F59">
+        <v>112.65838861589317</v>
+      </c>
+      <c r="G59">
+        <v>6</v>
+      </c>
+      <c r="H59">
+        <v>54.964329434025174</v>
+      </c>
+      <c r="I59">
+        <v>6543</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60">
@@ -1295,6 +2150,21 @@
       <c r="D60" t="str">
         <v>Female</v>
       </c>
+      <c r="E60">
+        <v>92.23517472165479</v>
+      </c>
+      <c r="F60">
+        <v>81.19740900196959</v>
+      </c>
+      <c r="G60">
+        <v>5</v>
+      </c>
+      <c r="H60">
+        <v>4.412292960692552</v>
+      </c>
+      <c r="I60">
+        <v>1338</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -1309,6 +2179,21 @@
       <c r="D61" t="str">
         <v>Female</v>
       </c>
+      <c r="E61">
+        <v>11.849918471380839</v>
+      </c>
+      <c r="F61">
+        <v>2.8291523048463496</v>
+      </c>
+      <c r="G61">
+        <v>5</v>
+      </c>
+      <c r="H61">
+        <v>68.36790982522876</v>
+      </c>
+      <c r="I61">
+        <v>1556</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -1323,6 +2208,21 @@
       <c r="D62" t="str">
         <v>Male</v>
       </c>
+      <c r="E62">
+        <v>69.56726331690908</v>
+      </c>
+      <c r="F62">
+        <v>181.18697275851468</v>
+      </c>
+      <c r="G62">
+        <v>2</v>
+      </c>
+      <c r="H62">
+        <v>4.171006925710499</v>
+      </c>
+      <c r="I62">
+        <v>625</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -1337,6 +2237,21 @@
       <c r="D63" t="str">
         <v>Female</v>
       </c>
+      <c r="E63">
+        <v>83.60656271323421</v>
+      </c>
+      <c r="F63">
+        <v>123.18828959258919</v>
+      </c>
+      <c r="G63">
+        <v>6</v>
+      </c>
+      <c r="H63">
+        <v>114.52083376424454</v>
+      </c>
+      <c r="I63">
+        <v>6643</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -1351,6 +2266,21 @@
       <c r="D64" t="str">
         <v>Male</v>
       </c>
+      <c r="E64">
+        <v>80.46452494509018</v>
+      </c>
+      <c r="F64">
+        <v>82.4520839744332</v>
+      </c>
+      <c r="G64">
+        <v>5</v>
+      </c>
+      <c r="H64">
+        <v>74.546501103384</v>
+      </c>
+      <c r="I64">
+        <v>5516</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -1365,6 +2295,21 @@
       <c r="D65" t="str">
         <v>Female</v>
       </c>
+      <c r="E65">
+        <v>23.87564402010771</v>
+      </c>
+      <c r="F65">
+        <v>166.55291068298794</v>
+      </c>
+      <c r="G65">
+        <v>2</v>
+      </c>
+      <c r="H65">
+        <v>8.563780028350028</v>
+      </c>
+      <c r="I65">
+        <v>70</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66">
@@ -1379,6 +2324,21 @@
       <c r="D66" t="str">
         <v>Male</v>
       </c>
+      <c r="E66">
+        <v>11.613672689859666</v>
+      </c>
+      <c r="F66">
+        <v>36.80331971141473</v>
+      </c>
+      <c r="G66">
+        <v>3</v>
+      </c>
+      <c r="H66">
+        <v>47.842551552990365</v>
+      </c>
+      <c r="I66">
+        <v>9580</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -1393,6 +2353,21 @@
       <c r="D67" t="str">
         <v>Female</v>
       </c>
+      <c r="E67">
+        <v>86.44683724785318</v>
+      </c>
+      <c r="F67">
+        <v>79.10023454604982</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>33.82651917219648</v>
+      </c>
+      <c r="I67">
+        <v>4136</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -1407,6 +2382,21 @@
       <c r="D68" t="str">
         <v>Male</v>
       </c>
+      <c r="E68">
+        <v>80.83364885038493</v>
+      </c>
+      <c r="F68">
+        <v>148.13273200466935</v>
+      </c>
+      <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="H68">
+        <v>23.73511790820439</v>
+      </c>
+      <c r="I68">
+        <v>6636</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69">
@@ -1421,6 +2411,21 @@
       <c r="D69" t="str">
         <v>Female</v>
       </c>
+      <c r="E69">
+        <v>14.941021682316237</v>
+      </c>
+      <c r="F69">
+        <v>14.816108082866375</v>
+      </c>
+      <c r="G69">
+        <v>3</v>
+      </c>
+      <c r="H69">
+        <v>18.154825021870835</v>
+      </c>
+      <c r="I69">
+        <v>5313</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70">
@@ -1435,6 +2440,21 @@
       <c r="D70" t="str">
         <v>Female</v>
       </c>
+      <c r="E70">
+        <v>93.93086874819896</v>
+      </c>
+      <c r="F70">
+        <v>178.0721809360617</v>
+      </c>
+      <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="H70">
+        <v>15.15751822717359</v>
+      </c>
+      <c r="I70">
+        <v>4969</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71">
@@ -1449,6 +2469,21 @@
       <c r="D71" t="str">
         <v>Male</v>
       </c>
+      <c r="E71">
+        <v>63.76992446067178</v>
+      </c>
+      <c r="F71">
+        <v>155.1291013967617</v>
+      </c>
+      <c r="G71">
+        <v>4</v>
+      </c>
+      <c r="H71">
+        <v>50.91991565709927</v>
+      </c>
+      <c r="I71">
+        <v>7256</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -1463,6 +2498,21 @@
       <c r="D72" t="str">
         <v>Female</v>
       </c>
+      <c r="E72">
+        <v>89.3685602436264</v>
+      </c>
+      <c r="F72">
+        <v>84.25028834940416</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>18.434792763296592</v>
+      </c>
+      <c r="I72">
+        <v>256</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -1477,6 +2527,21 @@
       <c r="D73" t="str">
         <v>Male</v>
       </c>
+      <c r="E73">
+        <v>3.7742275962005856</v>
+      </c>
+      <c r="F73">
+        <v>6.114245296049381</v>
+      </c>
+      <c r="G73">
+        <v>4</v>
+      </c>
+      <c r="H73">
+        <v>79.71243650387618</v>
+      </c>
+      <c r="I73">
+        <v>9131</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -1491,6 +2556,21 @@
       <c r="D74" t="str">
         <v>Female</v>
       </c>
+      <c r="E74">
+        <v>51.80049870775998</v>
+      </c>
+      <c r="F74">
+        <v>14.517676811482616</v>
+      </c>
+      <c r="G74">
+        <v>3</v>
+      </c>
+      <c r="H74">
+        <v>102.65854894219781</v>
+      </c>
+      <c r="I74">
+        <v>7629</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75">
@@ -1505,6 +2585,21 @@
       <c r="D75" t="str">
         <v>Male</v>
       </c>
+      <c r="E75">
+        <v>32.199839234790176</v>
+      </c>
+      <c r="F75">
+        <v>126.40693643619825</v>
+      </c>
+      <c r="G75">
+        <v>2</v>
+      </c>
+      <c r="H75">
+        <v>77.46923930007938</v>
+      </c>
+      <c r="I75">
+        <v>6089</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76">
@@ -1519,6 +2614,21 @@
       <c r="D76" t="str">
         <v>Female</v>
       </c>
+      <c r="E76">
+        <v>84.92392188642894</v>
+      </c>
+      <c r="F76">
+        <v>158.0687888749103</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>85.49373735564009</v>
+      </c>
+      <c r="I76">
+        <v>4108</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77">
@@ -1533,6 +2643,21 @@
       <c r="D77" t="str">
         <v>Female</v>
       </c>
+      <c r="E77">
+        <v>24.584089295945844</v>
+      </c>
+      <c r="F77">
+        <v>144.68898614393365</v>
+      </c>
+      <c r="G77">
+        <v>6</v>
+      </c>
+      <c r="H77">
+        <v>108.63432447222748</v>
+      </c>
+      <c r="I77">
+        <v>4058</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78">
@@ -1547,6 +2672,21 @@
       <c r="D78" t="str">
         <v>Male</v>
       </c>
+      <c r="E78">
+        <v>86.83138333403167</v>
+      </c>
+      <c r="F78">
+        <v>127.74777656108638</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>61.56934564343392</v>
+      </c>
+      <c r="I78">
+        <v>8655</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79">
@@ -1561,6 +2701,21 @@
       <c r="D79" t="str">
         <v>Female</v>
       </c>
+      <c r="E79">
+        <v>39.09437738522126</v>
+      </c>
+      <c r="F79">
+        <v>14.715615970093765</v>
+      </c>
+      <c r="G79">
+        <v>5</v>
+      </c>
+      <c r="H79">
+        <v>70.27124817396606</v>
+      </c>
+      <c r="I79">
+        <v>6725</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80">
@@ -1575,6 +2730,21 @@
       <c r="D80" t="str">
         <v>Female</v>
       </c>
+      <c r="E80">
+        <v>44.9012076116511</v>
+      </c>
+      <c r="F80">
+        <v>144.87744343296464</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <v>118.4111229144421</v>
+      </c>
+      <c r="I80">
+        <v>6841</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81">
@@ -1589,6 +2759,21 @@
       <c r="D81" t="str">
         <v>Male</v>
       </c>
+      <c r="E81">
+        <v>53.51435967029688</v>
+      </c>
+      <c r="F81">
+        <v>120.18637042882543</v>
+      </c>
+      <c r="G81">
+        <v>2</v>
+      </c>
+      <c r="H81">
+        <v>72.23917446533821</v>
+      </c>
+      <c r="I81">
+        <v>3308</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82">
@@ -1603,6 +2788,21 @@
       <c r="D82" t="str">
         <v>Female</v>
       </c>
+      <c r="E82">
+        <v>84.23013803727805</v>
+      </c>
+      <c r="F82">
+        <v>147.86606415329535</v>
+      </c>
+      <c r="G82">
+        <v>3</v>
+      </c>
+      <c r="H82">
+        <v>85.34483684128593</v>
+      </c>
+      <c r="I82">
+        <v>7046</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83">
@@ -1617,6 +2817,21 @@
       <c r="D83" t="str">
         <v>Female</v>
       </c>
+      <c r="E83">
+        <v>69.25392985476888</v>
+      </c>
+      <c r="F83">
+        <v>66.69972690688498</v>
+      </c>
+      <c r="G83">
+        <v>3</v>
+      </c>
+      <c r="H83">
+        <v>98.77475694389189</v>
+      </c>
+      <c r="I83">
+        <v>4110</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84">
@@ -1631,6 +2846,21 @@
       <c r="D84" t="str">
         <v>Male</v>
       </c>
+      <c r="E84">
+        <v>94.37471973248192</v>
+      </c>
+      <c r="F84">
+        <v>191.41865797791647</v>
+      </c>
+      <c r="G84">
+        <v>5</v>
+      </c>
+      <c r="H84">
+        <v>100.06991259311808</v>
+      </c>
+      <c r="I84">
+        <v>2549</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85">
@@ -1645,6 +2875,21 @@
       <c r="D85" t="str">
         <v>Female</v>
       </c>
+      <c r="E85">
+        <v>69.61169419995852</v>
+      </c>
+      <c r="F85">
+        <v>83.00682541963668</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>51.731489300384794</v>
+      </c>
+      <c r="I85">
+        <v>5174</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86">
@@ -1659,6 +2904,21 @@
       <c r="D86" t="str">
         <v>Male</v>
       </c>
+      <c r="E86">
+        <v>85.65874329665102</v>
+      </c>
+      <c r="F86">
+        <v>98.12271917633981</v>
+      </c>
+      <c r="G86">
+        <v>6</v>
+      </c>
+      <c r="H86">
+        <v>117.48266394865635</v>
+      </c>
+      <c r="I86">
+        <v>8231</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87">
@@ -1673,6 +2933,21 @@
       <c r="D87" t="str">
         <v>Male</v>
       </c>
+      <c r="E87">
+        <v>78.76782276205505</v>
+      </c>
+      <c r="F87">
+        <v>121.87537020738652</v>
+      </c>
+      <c r="G87">
+        <v>4</v>
+      </c>
+      <c r="H87">
+        <v>55.80115538055409</v>
+      </c>
+      <c r="I87">
+        <v>508</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88">
@@ -1687,6 +2962,21 @@
       <c r="D88" t="str">
         <v>Female</v>
       </c>
+      <c r="E88">
+        <v>34.35306763245085</v>
+      </c>
+      <c r="F88">
+        <v>101.8276416356135</v>
+      </c>
+      <c r="G88">
+        <v>6</v>
+      </c>
+      <c r="H88">
+        <v>28.15789252537286</v>
+      </c>
+      <c r="I88">
+        <v>5960</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89">
@@ -1701,6 +2991,21 @@
       <c r="D89" t="str">
         <v>Male</v>
       </c>
+      <c r="E89">
+        <v>35.0338815319373</v>
+      </c>
+      <c r="F89">
+        <v>29.981539338007536</v>
+      </c>
+      <c r="G89">
+        <v>3</v>
+      </c>
+      <c r="H89">
+        <v>119.89607738459375</v>
+      </c>
+      <c r="I89">
+        <v>8249</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90">
@@ -1715,6 +3020,21 @@
       <c r="D90" t="str">
         <v>Female</v>
       </c>
+      <c r="E90">
+        <v>79.09155965543306</v>
+      </c>
+      <c r="F90">
+        <v>135.14224790860294</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>7.756801021440269</v>
+      </c>
+      <c r="I90">
+        <v>8299</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91">
@@ -1729,6 +3049,21 @@
       <c r="D91" t="str">
         <v>Male</v>
       </c>
+      <c r="E91">
+        <v>30.42766494326632</v>
+      </c>
+      <c r="F91">
+        <v>58.36588918708112</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>36.685803999285085</v>
+      </c>
+      <c r="I91">
+        <v>9081</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92">
@@ -1743,6 +3078,21 @@
       <c r="D92" t="str">
         <v>Female</v>
       </c>
+      <c r="E92">
+        <v>62.03369167470232</v>
+      </c>
+      <c r="F92">
+        <v>112.7579427210363</v>
+      </c>
+      <c r="G92">
+        <v>5</v>
+      </c>
+      <c r="H92">
+        <v>14.413880524233544</v>
+      </c>
+      <c r="I92">
+        <v>3529</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93">
@@ -1757,6 +3107,21 @@
       <c r="D93" t="str">
         <v>Male</v>
       </c>
+      <c r="E93">
+        <v>29.560054061171503</v>
+      </c>
+      <c r="F93">
+        <v>101.3367787252673</v>
+      </c>
+      <c r="G93">
+        <v>4</v>
+      </c>
+      <c r="H93">
+        <v>9.983471300061577</v>
+      </c>
+      <c r="I93">
+        <v>399</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94">
@@ -1771,6 +3136,21 @@
       <c r="D94" t="str">
         <v>Female</v>
       </c>
+      <c r="E94">
+        <v>55.39581266432487</v>
+      </c>
+      <c r="F94">
+        <v>117.32852624503165</v>
+      </c>
+      <c r="G94">
+        <v>3</v>
+      </c>
+      <c r="H94">
+        <v>21.797593497740024</v>
+      </c>
+      <c r="I94">
+        <v>2352</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95">
@@ -1785,6 +3165,21 @@
       <c r="D95" t="str">
         <v>Male</v>
       </c>
+      <c r="E95">
+        <v>2.033139371934678</v>
+      </c>
+      <c r="F95">
+        <v>153.48615622917583</v>
+      </c>
+      <c r="G95">
+        <v>3</v>
+      </c>
+      <c r="H95">
+        <v>107.81422607904089</v>
+      </c>
+      <c r="I95">
+        <v>3401</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96">
@@ -1799,6 +3194,21 @@
       <c r="D96" t="str">
         <v>Female</v>
       </c>
+      <c r="E96">
+        <v>93.97591657595912</v>
+      </c>
+      <c r="F96">
+        <v>163.4368530201213</v>
+      </c>
+      <c r="G96">
+        <v>6</v>
+      </c>
+      <c r="H96">
+        <v>22.072850215774793</v>
+      </c>
+      <c r="I96">
+        <v>3732</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97">
@@ -1813,6 +3223,21 @@
       <c r="D97" t="str">
         <v>Male</v>
       </c>
+      <c r="E97">
+        <v>56.81604006882317</v>
+      </c>
+      <c r="F97">
+        <v>111.39734391290847</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <v>114.08695594485826</v>
+      </c>
+      <c r="I97">
+        <v>4445</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98">
@@ -1827,6 +3252,21 @@
       <c r="D98" t="str">
         <v>Female</v>
       </c>
+      <c r="E98">
+        <v>38.24204072747466</v>
+      </c>
+      <c r="F98">
+        <v>180.1626196778263</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>38.55632704948631</v>
+      </c>
+      <c r="I98">
+        <v>2633</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99">
@@ -1841,6 +3281,21 @@
       <c r="D99" t="str">
         <v>Female</v>
       </c>
+      <c r="E99">
+        <v>85.07770043308535</v>
+      </c>
+      <c r="F99">
+        <v>169.67337760548844</v>
+      </c>
+      <c r="G99">
+        <v>4</v>
+      </c>
+      <c r="H99">
+        <v>45.6297990280443</v>
+      </c>
+      <c r="I99">
+        <v>9117</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100">
@@ -1855,6 +3310,21 @@
       <c r="D100" t="str">
         <v>Male</v>
       </c>
+      <c r="E100">
+        <v>89.79698931166425</v>
+      </c>
+      <c r="F100">
+        <v>128.19670817027009</v>
+      </c>
+      <c r="G100">
+        <v>4</v>
+      </c>
+      <c r="H100">
+        <v>113.58441342109651</v>
+      </c>
+      <c r="I100">
+        <v>8545</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101">
@@ -1868,6 +3338,21 @@
       </c>
       <c r="D101" t="str">
         <v>Female</v>
+      </c>
+      <c r="E101">
+        <v>76.7872324219861</v>
+      </c>
+      <c r="F101">
+        <v>7.277633902805158</v>
+      </c>
+      <c r="G101">
+        <v>2</v>
+      </c>
+      <c r="H101">
+        <v>22.06791819253823</v>
+      </c>
+      <c r="I101">
+        <v>7704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding data to xlsx
</commit_message>
<xml_diff>
--- a/server/Fitness_Records_Hackathon.xlsx
+++ b/server/Fitness_Records_Hackathon.xlsx
@@ -468,20 +468,20 @@
       <c r="D2" t="str">
         <v>Female</v>
       </c>
-      <c r="E2">
-        <v>20.529902773642704</v>
-      </c>
-      <c r="F2">
-        <v>47.831146818906234</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>96.3671244523385</v>
-      </c>
-      <c r="I2">
-        <v>7607</v>
+      <c r="E2" t="str">
+        <v>89</v>
+      </c>
+      <c r="F2" t="str">
+        <v>134</v>
+      </c>
+      <c r="G2" t="str">
+        <v>5</v>
+      </c>
+      <c r="H2" t="str">
+        <v>2</v>
+      </c>
+      <c r="I2" t="str">
+        <v>10000</v>
       </c>
     </row>
     <row r="3">

</xml_diff>